<commit_message>
ajout du changement de position en fonction de la coueur du joueur
</commit_message>
<xml_diff>
--- a/Plateau.xlsx
+++ b/Plateau.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\Documents\Prog\ISNEchecs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Code\Git\ISNEchecs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -33,10 +33,23 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -51,7 +64,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -83,12 +96,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -109,7 +125,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -373,11 +389,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="280" zoomScaleNormal="280" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="6.7109375" defaultRowHeight="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
@@ -392,7 +408,7 @@
       <c r="D1" s="1">
         <v>3</v>
       </c>
-      <c r="E1" s="1">
+      <c r="E1" s="2">
         <v>4</v>
       </c>
       <c r="F1" s="1">
@@ -435,7 +451,7 @@
       <c r="A3" s="1">
         <v>16</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="3">
         <v>17</v>
       </c>
       <c r="C3" s="1">
@@ -450,7 +466,7 @@
       <c r="F3" s="1">
         <v>21</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G3" s="3">
         <v>22</v>
       </c>
       <c r="H3" s="1">
@@ -565,7 +581,7 @@
       </c>
     </row>
     <row r="8" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
+      <c r="A8" s="2">
         <v>56</v>
       </c>
       <c r="B8" s="1">
@@ -592,5 +608,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>